<commit_message>
adding day/night for Cousins10
</commit_message>
<xml_diff>
--- a/analyses/alternatingTempPaperList.xlsx
+++ b/analyses/alternatingTempPaperList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapph\Documents\ubc things\work\egret\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92A61680-2599-4FC2-AF65-9C4AE7A69C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4285C75F-1CB6-46A2-9055-91C6053E9EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{982251BE-C79F-432A-A20B-D9A10B810B6B}"/>
   </bookViews>
@@ -1953,17 +1953,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <font>
-        <color theme="3" tint="9.9948118533890809E-2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1986,181 +1976,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color theme="3" tint="9.9948118533890809E-2"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2507,8 +2327,8 @@
   <dimension ref="A1:H300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G119" sqref="G119"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4238,8 +4058,8 @@
       <c r="E85" t="s">
         <v>15</v>
       </c>
-      <c r="H85" t="s">
-        <v>24</v>
+      <c r="F85" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
@@ -7800,7 +7620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="257" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>262</v>
       </c>
@@ -8714,20 +8534,22 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="H244:H246 G299 F301:F1048576 F300:G300 F1:F299">
-    <cfRule type="containsText" dxfId="12" priority="8" operator="containsText" text="constant">
+  <conditionalFormatting sqref="F1:F299 G299 F300:G300 F301:F1048576 H244:H246">
+    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="constant">
       <formula>NOT(ISERROR(SEARCH("constant",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="altern">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F299 G299 F300:G300 F301:F1048576">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"ambient"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F299 H244:H246 G299 F300:G300 F301:F1048576">
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="altern">
       <formula>NOT(ISERROR(SEARCH("altern",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="night/day">
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="night/day">
       <formula>NOT(ISERROR(SEARCH("night/day",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G299 F301:F1048576 F300:G300 F1:F299">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"ambient"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on the alternating temp papers
</commit_message>
<xml_diff>
--- a/analyses/alternatingTempPaperList.xlsx
+++ b/analyses/alternatingTempPaperList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapph\Documents\ubc things\work\egret\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4285C75F-1CB6-46A2-9055-91C6053E9EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AFDAA4-61EA-4054-9789-F9C999951298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{982251BE-C79F-432A-A20B-D9A10B810B6B}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1577" uniqueCount="471">
   <si>
     <t>datasetID</t>
   </si>
@@ -1418,7 +1418,22 @@
     <t>ambient</t>
   </si>
   <si>
-    <t>alternation or range?</t>
+    <t>new column entry</t>
+  </si>
+  <si>
+    <t>constant light/constant dark</t>
+  </si>
+  <si>
+    <t>""/constant dark</t>
+  </si>
+  <si>
+    <t>NEED CLARIFICATION</t>
+  </si>
+  <si>
+    <t>no photoperiod specified</t>
+  </si>
+  <si>
+    <t>photoperiod is 15 but the actual temperature alternation is 12</t>
   </si>
 </sst>
 </file>
@@ -1953,7 +1968,57 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3" tint="9.9948118533890809E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2324,11 +2389,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61ACE8D6-BECD-46AB-A6DD-BAA417D27839}">
-  <dimension ref="A1:H300"/>
+  <dimension ref="A1:I300"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2336,9 +2401,10 @@
     <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2360,8 +2426,11 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2381,7 +2450,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2403,8 +2472,11 @@
       <c r="G3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2426,8 +2498,11 @@
       <c r="G4" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2449,8 +2524,11 @@
       <c r="G5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2470,7 +2548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2490,7 +2568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2510,7 +2588,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2530,7 +2608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2550,7 +2628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2570,7 +2648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2590,7 +2668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2610,7 +2688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2630,7 +2708,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2650,7 +2728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2832,8 +2910,11 @@
       <c r="E24" t="s">
         <v>15</v>
       </c>
-      <c r="H24" t="s">
-        <v>24</v>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2852,8 +2933,11 @@
       <c r="E25" t="s">
         <v>10</v>
       </c>
-      <c r="H25" t="s">
-        <v>24</v>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2872,8 +2956,11 @@
       <c r="E26" t="s">
         <v>19</v>
       </c>
-      <c r="H26" t="s">
-        <v>24</v>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -2892,8 +2979,11 @@
       <c r="E27" t="s">
         <v>25</v>
       </c>
-      <c r="H27" t="s">
-        <v>24</v>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -4602,7 +4692,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4622,7 +4712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4638,11 +4728,14 @@
       <c r="E114" t="s">
         <v>15</v>
       </c>
-      <c r="H114" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F114" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>120</v>
       </c>
@@ -4662,7 +4755,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>121</v>
       </c>
@@ -4682,7 +4775,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>122</v>
       </c>
@@ -4702,7 +4795,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>123</v>
       </c>
@@ -4722,7 +4815,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>124</v>
       </c>
@@ -4742,7 +4835,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>125</v>
       </c>
@@ -4762,7 +4855,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>126</v>
       </c>
@@ -4782,7 +4875,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>127</v>
       </c>
@@ -4802,7 +4895,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>128</v>
       </c>
@@ -4822,7 +4915,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>129</v>
       </c>
@@ -4842,7 +4935,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>130</v>
       </c>
@@ -4862,7 +4955,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>131</v>
       </c>
@@ -4882,7 +4975,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>132</v>
       </c>
@@ -4902,7 +4995,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>133</v>
       </c>
@@ -6256,7 +6349,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>198</v>
       </c>
@@ -6276,7 +6369,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>199</v>
       </c>
@@ -6296,7 +6389,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>200</v>
       </c>
@@ -6316,7 +6409,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>201</v>
       </c>
@@ -6336,7 +6429,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>202</v>
       </c>
@@ -6356,7 +6449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>203</v>
       </c>
@@ -6376,7 +6469,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>204</v>
       </c>
@@ -6396,7 +6489,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>205</v>
       </c>
@@ -6416,7 +6509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>206</v>
       </c>
@@ -6436,7 +6529,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>207</v>
       </c>
@@ -6459,7 +6552,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>208</v>
       </c>
@@ -6481,8 +6574,11 @@
       <c r="H203" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I203" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>209</v>
       </c>
@@ -6502,7 +6598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>210</v>
       </c>
@@ -6522,7 +6618,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>211</v>
       </c>
@@ -6542,7 +6638,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>212</v>
       </c>
@@ -6562,7 +6658,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>213</v>
       </c>
@@ -7946,7 +8042,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="273" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>278</v>
       </c>
@@ -7966,7 +8062,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="274" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>279</v>
       </c>
@@ -7986,7 +8082,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="275" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>280</v>
       </c>
@@ -8006,7 +8102,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="276" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>281</v>
       </c>
@@ -8028,8 +8124,11 @@
       <c r="G276" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="277" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I276" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>282</v>
       </c>
@@ -8049,7 +8148,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="278" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>283</v>
       </c>
@@ -8069,7 +8168,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="279" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>284</v>
       </c>
@@ -8089,7 +8188,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="280" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>285</v>
       </c>
@@ -8112,7 +8211,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="281" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>286</v>
       </c>
@@ -8135,7 +8234,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="282" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>287</v>
       </c>
@@ -8158,7 +8257,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="283" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>288</v>
       </c>
@@ -8181,7 +8280,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>289</v>
       </c>
@@ -8204,7 +8303,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="285" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>290</v>
       </c>
@@ -8227,7 +8326,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="286" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>291</v>
       </c>
@@ -8247,7 +8346,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="287" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>292</v>
       </c>
@@ -8267,7 +8366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="288" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>293</v>
       </c>
@@ -8324,7 +8423,7 @@
         <v>15</v>
       </c>
       <c r="H290" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.3">
@@ -8534,22 +8633,27 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:F299 G299 F300:G300 F301:F1048576 H244:H246">
-    <cfRule type="containsText" dxfId="3" priority="8" operator="containsText" text="constant">
+  <conditionalFormatting sqref="G299 F300:G300 F301:F1048576 H244:H246 F1:F299">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="constant">
       <formula>NOT(ISERROR(SEARCH("constant",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F299 G299 F300:G300 F301:F1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+  <conditionalFormatting sqref="G299 F300:G300 F301:F1048576 F1:F299">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"ambient"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1:F299 H244:H246 G299 F300:G300 F301:F1048576">
-    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="altern">
+  <conditionalFormatting sqref="H244:H246 G299 F300:G300 F301:F1048576 F1:F299">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="altern">
       <formula>NOT(ISERROR(SEARCH("altern",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="night/day">
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="night/day">
       <formula>NOT(ISERROR(SEARCH("night/day",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:G1048576 H290">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="OR">
+      <formula>NOT(ISERROR(SEARCH("OR",G1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>